<commit_message>
From dell move project to Open Server 5.4.3
</commit_message>
<xml_diff>
--- a/api/Архитектура БД superjob.xlsx
+++ b/api/Архитектура БД superjob.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROGRAMS\OSPanel2022\domains\superjob\api\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38670" windowHeight="12195" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12192"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
     <sheet name="chat" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -231,8 +226,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,7 +410,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -450,7 +445,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -627,35 +622,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:AB22"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="16" max="20" width="14.28515625" customWidth="1"/>
-    <col min="21" max="21" width="10.7109375" customWidth="1"/>
-    <col min="22" max="22" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.44140625" customWidth="1"/>
+    <col min="16" max="20" width="14.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
+    <col min="22" max="22" width="12.109375" customWidth="1"/>
     <col min="23" max="23" width="12" customWidth="1"/>
-    <col min="24" max="24" width="12.28515625" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" customWidth="1"/>
-    <col min="26" max="26" width="13.140625" customWidth="1"/>
+    <col min="24" max="24" width="12.33203125" customWidth="1"/>
+    <col min="25" max="25" width="11.88671875" customWidth="1"/>
+    <col min="26" max="26" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:28" s="7" customFormat="1">
       <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
@@ -666,7 +661,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="2:28" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:28" s="7" customFormat="1">
       <c r="B2" s="7" t="s">
         <v>27</v>
       </c>
@@ -722,7 +717,7 @@
         <v>28</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>39</v>
@@ -740,7 +735,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:28">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -815,7 +810,7 @@
       </c>
       <c r="AB3" s="5"/>
     </row>
-    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:28">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -855,7 +850,7 @@
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
     </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:28">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -895,7 +890,7 @@
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
     </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -935,7 +930,7 @@
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
     </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -975,7 +970,7 @@
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
     </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -1015,7 +1010,7 @@
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:28">
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1055,7 +1050,7 @@
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
     </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:28">
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1095,7 +1090,7 @@
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
     </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:28">
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1135,7 +1130,7 @@
       <c r="Z11" s="1"/>
       <c r="AA11" s="1"/>
     </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:28">
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1170,7 @@
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
     </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:28">
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1192,7 +1187,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:28">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1225,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17">
       <c r="B17" s="4">
         <v>6</v>
       </c>
@@ -1268,7 +1263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17">
       <c r="B18" s="4">
         <v>10</v>
       </c>
@@ -1294,7 +1289,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17">
       <c r="B19" s="4">
         <v>12</v>
       </c>
@@ -1320,7 +1315,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17">
       <c r="B20" s="4">
         <v>13</v>
       </c>
@@ -1340,7 +1335,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" s="4">
         <v>7</v>
       </c>
@@ -1354,7 +1349,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" s="4">
         <v>9</v>
       </c>
@@ -1369,22 +1364,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="355" zoomScaleNormal="355" workbookViewId="0">
+    <sheetView zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10">
       <c r="B1" s="8" t="s">
         <v>59</v>
       </c>
@@ -1401,7 +1396,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10">
       <c r="B2" s="8" t="s">
         <v>58</v>
       </c>
@@ -1418,7 +1413,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10">
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1439,13 +1434,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1454,7 +1449,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1463,7 +1458,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -1475,7 +1470,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="F8" s="13" t="s">
         <v>66</v>
       </c>
@@ -1492,52 +1487,52 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="E9" s="11"/>
       <c r="F9" s="15"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10">
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10">
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10">
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10">
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10">
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:7">
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:7">
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>

</xml_diff>